<commit_message>
final polygon generator, completed
</commit_message>
<xml_diff>
--- a/PolygonOrientation.xlsx
+++ b/PolygonOrientation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\PolygonOrientationFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F99A6A-A6C5-438E-9517-CB6C5A926B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4D799B-E2D0-45D5-AF14-179E065A606A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00F95ED5-E64E-4F00-B2FF-8249EB2D7511}"/>
   </bookViews>
@@ -194,7 +194,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{629D5B6C-2AF1-4F55-88A8-00643E15A86A}" type="CELLRANGE">
+                    <a:fld id="{4B436650-D97E-451D-9116-60A5A101A367}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -228,7 +228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA39D645-710F-42E4-9809-3545BDF9E0E3}" type="CELLRANGE">
+                    <a:fld id="{49F6695C-BE07-4825-81E2-4EEE23297968}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -262,7 +262,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDD84A0C-C105-40B7-877F-668078E2B65B}" type="CELLRANGE">
+                    <a:fld id="{C1A60131-5228-40A9-AFA9-3C684268E343}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -296,7 +296,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{345B94DF-4C4E-4301-B9B9-024418908F21}" type="CELLRANGE">
+                    <a:fld id="{F2AB7EDC-35B8-4C0B-A39C-7759D5331DD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -330,7 +330,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63D561E1-0F11-4236-B992-2A1287330C24}" type="CELLRANGE">
+                    <a:fld id="{46F5C097-3E68-4B10-8A3F-29E0B8FF0E06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -364,7 +364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D94EEDF3-FC4A-41BB-BE6D-7A577A2B901E}" type="CELLRANGE">
+                    <a:fld id="{8D9937F6-C109-420F-9B8A-92A2DA381143}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -398,7 +398,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1A79C87-5EB8-410C-97E4-329D5273CDA5}" type="CELLRANGE">
+                    <a:fld id="{E23807C4-ADF7-40DE-9AF6-35D96B131F78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -432,7 +432,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0DFAEEF-2F41-47C1-B57F-013AA71D8803}" type="CELLRANGE">
+                    <a:fld id="{5321EF53-4614-49C2-BCC0-299AF188EE75}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -466,7 +466,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4489C515-6952-4DEF-95CA-870EC39187A1}" type="CELLRANGE">
+                    <a:fld id="{79A24B21-7C81-4ADA-9413-AFE911C7117F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -500,7 +500,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2E8C0B9-5B36-4956-B0CB-1391DBC51995}" type="CELLRANGE">
+                    <a:fld id="{D3640F04-7FCC-4EA0-91B2-D8EFE1DDB22B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -980,7 +980,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{660C6F8B-ECF5-429C-AE8E-98E574B85456}" type="CELLRANGE">
+                    <a:fld id="{2CD6CBD0-7E6A-4AAF-B131-C596CB2EB844}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1014,7 +1014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{096E51BA-7504-4D98-8B54-F982FC20F102}" type="CELLRANGE">
+                    <a:fld id="{7373C0DD-F737-46A9-9A75-CE75B1796117}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1054,7 +1054,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A99E5E28-48F4-4A47-BE93-C3EC5152A551}" type="CELLRANGE">
+                    <a:fld id="{792AE1E6-5FA7-4505-ACF0-01B62E8AE5B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1087,7 +1087,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{63BBBD52-B172-4708-B9F3-513399B59A51}" type="CELLRANGE">
+                    <a:fld id="{CA001F5B-D7FA-45F0-9123-761DD9E08AF0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1121,7 +1121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3163BDBF-6A97-4D86-8E0B-51CEAC182A06}" type="CELLRANGE">
+                    <a:fld id="{7CC84328-D68F-4EA1-B462-C9BD395FB300}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1155,7 +1155,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFCE17B1-9BA0-4008-9DB4-EB7209B103C8}" type="CELLRANGE">
+                    <a:fld id="{8E612802-6D5A-420D-978F-1906DFAF8808}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1195,7 +1195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C9CA517-F089-432C-A633-BE91C90F846A}" type="CELLRANGE">
+                    <a:fld id="{F9D34F6D-9E0F-4D64-AF1D-FF1BEDAD8CCA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1228,7 +1228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6521D0BB-A362-47A2-9B46-F8F4A4A72A63}" type="CELLRANGE">
+                    <a:fld id="{284688D2-9CA7-4B61-AC16-C37432E25604}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1268,7 +1268,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64C9143C-8CAA-4EC3-9859-2760A22DB6DA}" type="CELLRANGE">
+                    <a:fld id="{3477272D-6A7C-4ED8-BAC8-BDA19335E395}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1301,7 +1301,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73509D85-860B-4F84-B41B-DDD75F5069AC}" type="CELLRANGE">
+                    <a:fld id="{F9159D7D-7029-407F-ACC1-D8630CB28EDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1341,7 +1341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72449CAB-0A34-40D5-A86E-537AB7A01277}" type="CELLRANGE">
+                    <a:fld id="{A5D11832-0A59-41C6-80A5-2EFA99E21DF4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1374,7 +1374,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8CD39C5-B34A-47B5-AC6C-D263BDA3ABAF}" type="CELLRANGE">
+                    <a:fld id="{352EFD06-58B9-4B16-984E-CF514933FF14}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1408,7 +1408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C4718D2-D9A3-423F-AD6E-63503DF6CEBD}" type="CELLRANGE">
+                    <a:fld id="{8AF03A72-35A2-4F83-A77B-2A7733D33913}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1448,7 +1448,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29ABA43E-EC76-4855-BB30-01C80C2CC84E}" type="CELLRANGE">
+                    <a:fld id="{2CD3C5A7-687D-432C-B36A-CC1E216D173D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1572,7 +1572,7 @@
                   <c:v>3.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.58</c:v>
+                  <c:v>5.58</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.53</c:v>
@@ -3372,7 +3372,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="A1:XFD1048576"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,7 +3498,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,7 +3629,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>7.58</v>
+        <v>5.58</v>
       </c>
       <c r="C12">
         <v>-3.5</v>

</xml_diff>